<commit_message>
get faturas and insert to efaturas portal
</commit_message>
<xml_diff>
--- a/listagem/teste.xlsx
+++ b/listagem/teste.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Scripts\Python\efaturas-automate\listagem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62598CAB-5FEB-430E-93C4-F60618B86966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE246223-B39F-48D6-B340-44E4EA440203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1155" windowWidth="28770" windowHeight="15375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="21600" windowHeight="11145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>NUMERO</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>VALOR</t>
+  </si>
+  <si>
+    <t>5,9</t>
   </si>
 </sst>
 </file>
@@ -364,7 +367,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -398,7 +401,7 @@
         <v>44574</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>20.7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -412,7 +415,7 @@
         <v>44575</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -439,8 +442,8 @@
       <c r="C5" s="1">
         <v>44577</v>
       </c>
-      <c r="D5">
-        <v>5</v>
+      <c r="D5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>